<commit_message>
added more demo files
added more educational demo files
</commit_message>
<xml_diff>
--- a/Bike Sales/XLOOKUP Excel Tutorial File.xlsx
+++ b/Bike Sales/XLOOKUP Excel Tutorial File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_repo\excel_project_portfolio\Bike Sales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_repo\excel_project_portfolio\excel_portfolio_projects\Bike Sales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870D5176-C9C5-43BE-8894-023BD379FF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90284F9E-C900-4DC5-BBCF-98A47A3F9F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{5EA44D8F-79D3-45F5-A0F6-C7F47358B7ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="6" xr2:uid="{5EA44D8F-79D3-45F5-A0F6-C7F47358B7ED}"/>
   </bookViews>
   <sheets>
     <sheet name="XLookUp" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="100">
   <si>
     <t>EmployeeID</t>
   </si>
@@ -353,6 +353,15 @@
   </si>
   <si>
     <t>searches last to first</t>
+  </si>
+  <si>
+    <t>sum of 2 xlookups</t>
+  </si>
+  <si>
+    <t>xlookups horizontally rather than column</t>
+  </si>
+  <si>
+    <t>vlookup uses a number to indicate which column to look for value from starting from the first highlighted column. Bad because if add another column, need to change the column index. Xlookup superior</t>
   </si>
 </sst>
 </file>
@@ -2416,197 +2425,6 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CCAA7F-6F85-4102-B7D4-D80770622F9F}">
-  <dimension ref="A1:S4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L1" t="s">
-        <v>76</v>
-      </c>
-      <c r="M1" t="s">
-        <v>77</v>
-      </c>
-      <c r="N1" t="s">
-        <v>78</v>
-      </c>
-      <c r="O1" t="s">
-        <v>79</v>
-      </c>
-      <c r="P1" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>81</v>
-      </c>
-      <c r="R1" t="s">
-        <v>82</v>
-      </c>
-      <c r="S1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2">
-        <v>450</v>
-      </c>
-      <c r="I2">
-        <v>310</v>
-      </c>
-      <c r="J2">
-        <v>150</v>
-      </c>
-      <c r="K2">
-        <v>750</v>
-      </c>
-      <c r="L2">
-        <v>440</v>
-      </c>
-      <c r="M2">
-        <v>485</v>
-      </c>
-      <c r="N2">
-        <v>510</v>
-      </c>
-      <c r="O2">
-        <v>347</v>
-      </c>
-      <c r="P2">
-        <v>736</v>
-      </c>
-      <c r="Q2">
-        <v>155</v>
-      </c>
-      <c r="R2">
-        <v>450</v>
-      </c>
-      <c r="S2">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G3" t="s">
-        <v>71</v>
-      </c>
-      <c r="H3">
-        <v>75</v>
-      </c>
-      <c r="I3">
-        <v>40</v>
-      </c>
-      <c r="J3">
-        <v>65</v>
-      </c>
-      <c r="K3">
-        <v>50</v>
-      </c>
-      <c r="L3">
-        <v>24</v>
-      </c>
-      <c r="M3">
-        <v>71</v>
-      </c>
-      <c r="N3">
-        <v>57</v>
-      </c>
-      <c r="O3">
-        <v>61</v>
-      </c>
-      <c r="P3">
-        <v>34</v>
-      </c>
-      <c r="Q3">
-        <v>41</v>
-      </c>
-      <c r="R3">
-        <v>58</v>
-      </c>
-      <c r="S3">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H4">
-        <v>200</v>
-      </c>
-      <c r="I4">
-        <v>118</v>
-      </c>
-      <c r="J4">
-        <v>145</v>
-      </c>
-      <c r="K4">
-        <v>210</v>
-      </c>
-      <c r="L4">
-        <v>45</v>
-      </c>
-      <c r="M4">
-        <v>170</v>
-      </c>
-      <c r="N4">
-        <v>130</v>
-      </c>
-      <c r="O4">
-        <v>90</v>
-      </c>
-      <c r="P4">
-        <v>55</v>
-      </c>
-      <c r="Q4">
-        <v>110</v>
-      </c>
-      <c r="R4">
-        <v>130</v>
-      </c>
-      <c r="S4">
-        <v>180</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A2549A4-3A41-4806-B7FD-3B9C6823775F}">
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2663,6 +2481,10 @@
       <c r="A2" t="s">
         <v>70</v>
       </c>
+      <c r="B2">
+        <f>_xlfn.XLOOKUP(I1,H1:S1,H2:S2)</f>
+        <v>310</v>
+      </c>
       <c r="G2" t="s">
         <v>70</v>
       </c>
@@ -2707,6 +2529,10 @@
       <c r="A3" t="s">
         <v>71</v>
       </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B4" si="0">_xlfn.XLOOKUP(I2,H2:S2,H3:S3)</f>
+        <v>40</v>
+      </c>
       <c r="G3" t="s">
         <v>71</v>
       </c>
@@ -2751,6 +2577,218 @@
       <c r="A4" t="s">
         <v>84</v>
       </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>118</v>
+      </c>
+      <c r="G4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4">
+        <v>200</v>
+      </c>
+      <c r="I4">
+        <v>118</v>
+      </c>
+      <c r="J4">
+        <v>145</v>
+      </c>
+      <c r="K4">
+        <v>210</v>
+      </c>
+      <c r="L4">
+        <v>45</v>
+      </c>
+      <c r="M4">
+        <v>170</v>
+      </c>
+      <c r="N4">
+        <v>130</v>
+      </c>
+      <c r="O4">
+        <v>90</v>
+      </c>
+      <c r="P4">
+        <v>55</v>
+      </c>
+      <c r="Q4">
+        <v>110</v>
+      </c>
+      <c r="R4">
+        <v>130</v>
+      </c>
+      <c r="S4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A2549A4-3A41-4806-B7FD-3B9C6823775F}">
+  <dimension ref="A1:S7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O1" t="s">
+        <v>79</v>
+      </c>
+      <c r="P1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>81</v>
+      </c>
+      <c r="R1" t="s">
+        <v>82</v>
+      </c>
+      <c r="S1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2">
+        <f>_xlfn.XLOOKUP(I1,H1:S1,H2:S2)</f>
+        <v>310</v>
+      </c>
+      <c r="G2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2">
+        <v>450</v>
+      </c>
+      <c r="I2">
+        <v>310</v>
+      </c>
+      <c r="J2">
+        <v>150</v>
+      </c>
+      <c r="K2">
+        <v>750</v>
+      </c>
+      <c r="L2">
+        <v>440</v>
+      </c>
+      <c r="M2">
+        <v>485</v>
+      </c>
+      <c r="N2">
+        <v>510</v>
+      </c>
+      <c r="O2">
+        <v>347</v>
+      </c>
+      <c r="P2">
+        <v>736</v>
+      </c>
+      <c r="Q2">
+        <v>155</v>
+      </c>
+      <c r="R2">
+        <v>450</v>
+      </c>
+      <c r="S2">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B4" si="0">_xlfn.XLOOKUP(I2,H2:S2,H3:S3)</f>
+        <v>40</v>
+      </c>
+      <c r="G3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3">
+        <v>75</v>
+      </c>
+      <c r="I3">
+        <v>40</v>
+      </c>
+      <c r="J3">
+        <v>65</v>
+      </c>
+      <c r="K3">
+        <v>50</v>
+      </c>
+      <c r="L3">
+        <v>24</v>
+      </c>
+      <c r="M3">
+        <v>71</v>
+      </c>
+      <c r="N3">
+        <v>57</v>
+      </c>
+      <c r="O3">
+        <v>61</v>
+      </c>
+      <c r="P3">
+        <v>34</v>
+      </c>
+      <c r="Q3">
+        <v>41</v>
+      </c>
+      <c r="R3">
+        <v>58</v>
+      </c>
+      <c r="S3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>118</v>
+      </c>
       <c r="G4" t="s">
         <v>84</v>
       </c>
@@ -2799,6 +2837,13 @@
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>70</v>
+      </c>
+      <c r="B7">
+        <f>SUM(_xlfn.XLOOKUP(I1,H1:S1,H2:S2):_xlfn.XLOOKUP(J1,H1:S1,H2:S2))</f>
+        <v>460</v>
+      </c>
+      <c r="D7" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2808,10 +2853,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F9C169-12D8-441E-870D-6C6EF0F6521C}">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2902,6 +2947,10 @@
       <c r="A3" t="s">
         <v>63</v>
       </c>
+      <c r="B3" t="str">
+        <f>VLOOKUP(A3,H2:P10, 9,FALSE)</f>
+        <v>Dwight.Schrute@AOL.com</v>
+      </c>
       <c r="E3">
         <v>1002</v>
       </c>
@@ -2940,6 +2989,10 @@
       <c r="A4" t="s">
         <v>66</v>
       </c>
+      <c r="B4" t="str">
+        <f t="shared" ref="B4:B5" si="0">VLOOKUP(A4,H3:P11, 9,FALSE)</f>
+        <v>Michael.Scott@DunderMifflin.com</v>
+      </c>
       <c r="E4">
         <v>1003</v>
       </c>
@@ -2978,6 +3031,10 @@
       <c r="A5" t="s">
         <v>68</v>
       </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>Stanley.Hudson@gmail.com</v>
+      </c>
       <c r="E5">
         <v>1004</v>
       </c>
@@ -3185,6 +3242,11 @@
       </c>
       <c r="P10" s="2" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>